<commit_message>
Improved Readme and added documents
+ Added documents with calculate Tanabe-Sugano diagrams, crystal field matrix elements, coupling coefficients, and spin-orbital wavefunctions.
+ HartreeFockData acknowledges the source of data to Fraga's handbook.
+ Small update to conversion factors.
+ Improved qdef.ipynb.
</commit_message>
<xml_diff>
--- a/qdef/data/ConversionFactors.xlsx
+++ b/qdef/data/ConversionFactors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Zia Lab/Codebase/qdef/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/ZiaLab/Codebase/qdef/qdef/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61316395-B191-9644-9E1D-34EA7E71BE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126C07A6-BC46-474E-B0FE-A4F3AF250EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28000" windowHeight="18000" activeTab="5" xr2:uid="{AAAE55A6-0C68-0541-BB78-4F67D14A1699}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28000" windowHeight="18000" activeTab="2" xr2:uid="{AAAE55A6-0C68-0541-BB78-4F67D14A1699}"/>
   </bookViews>
   <sheets>
     <sheet name="time" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="128">
   <si>
     <t>m</t>
   </si>
@@ -417,6 +417,12 @@
   </si>
   <si>
     <t>miligauss</t>
+  </si>
+  <si>
+    <t>cm^-1</t>
+  </si>
+  <si>
+    <t>inverse cm</t>
   </si>
 </sst>
 </file>
@@ -1257,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE195A5-F53F-094E-B172-A5DC4E7C6C13}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1606,6 +1612,23 @@
       </c>
       <c r="E20" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="1">
+        <v>8065.5442899999998</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1790,7 +1813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B73242FA-81F1-4D4B-A13C-538CA1BBD2D4}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>